<commit_message>
Fix handing of boolean fields (wordbool rather then boolean)
</commit_message>
<xml_diff>
--- a/demos/TestData.xlsx
+++ b/demos/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">IntCol</t>
   </si>
@@ -40,34 +40,25 @@
     <t xml:space="preserve">1</t>
   </si>
   <si>
+    <t xml:space="preserve">def</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ghi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abc</t>
+  </si>
+  <si>
     <t xml:space="preserve">true</t>
   </si>
   <si>
-    <t xml:space="preserve">def</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ghi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">true</t>
-  </si>
-  <si>
     <t xml:space="preserve">jkl</t>
   </si>
   <si>
     <t xml:space="preserve">12345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">false</t>
   </si>
   <si>
     <t xml:space="preserve">mno</t>
@@ -245,8 +236,8 @@
       <c r="E2" s="1" t="n">
         <v>44228</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>8</v>
+      <c r="F2" s="0" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -254,10 +245,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>10</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>2.2</v>
@@ -265,8 +256,8 @@
       <c r="E3" s="1" t="n">
         <v>44229</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>11</v>
+      <c r="F3" s="0" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -274,10 +265,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>3.29999977111816</v>
@@ -286,7 +277,7 @@
         <v>44230</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -294,10 +285,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>4.39999771118164</v>
@@ -305,8 +296,8 @@
       <c r="E5" s="1" t="n">
         <v>44231</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>17</v>
+      <c r="F5" s="0" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -314,10 +305,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>5.5</v>
@@ -326,7 +317,7 @@
         <v>44232</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -334,10 +325,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>6.6</v>
@@ -346,7 +337,7 @@
         <v>44233</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -357,7 +348,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>7.7</v>
@@ -366,7 +357,7 @@
         <v>44234</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -374,10 +365,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>8.8</v>
@@ -386,7 +377,7 @@
         <v>44235</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -394,10 +385,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>9.9</v>
@@ -406,7 +397,7 @@
         <v>44236</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -417,7 +408,7 @@
         <v>433</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>10.1</v>
@@ -426,7 +417,7 @@
         <v>44237</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -434,10 +425,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>11.11</v>
@@ -446,7 +437,7 @@
         <v>44238</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -454,7 +445,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>12.22</v>
@@ -463,7 +454,7 @@
         <v>44239</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Support field data type ftCurrency.
</commit_message>
<xml_diff>
--- a/demos/TestData.xlsx
+++ b/demos/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">IntCol</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">BoolCol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CurrencyCol</t>
   </si>
   <si>
     <t xml:space="preserve">abc</t>
@@ -101,6 +104,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$$]* #,##0.00;[$$]* &quot;-&quot;#,##0.00&quot; &quot;;[$$]* &quot;-&quot;??;@"/>
+    <numFmt numFmtId="165" formatCode="0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -143,9 +150,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" xfId="0"/>
     <xf numFmtId="14" applyNumberFormat="1" fontId="0" xfId="0"/>
+    <xf numFmtId="164" applyNumberFormat="1" fontId="0" xfId="0"/>
+    <xf numFmtId="165" applyNumberFormat="1" fontId="0" xfId="0"/>
+    <xf numFmtId="7" applyNumberFormat="1" fontId="0" xfId="0"/>
+    <xf numFmtId="7" applyNumberFormat="1" fontId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,10 +168,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1" rightToLeft="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.14" defaultRowHeight="15.00" customHeight="true"/>
@@ -171,9 +182,10 @@
     <col min="4" max="4" width="9.14"/>
     <col min="5" max="5" width="20.14" customWidth="1"/>
     <col min="6" max="6" width="9.14"/>
+    <col min="7" max="7" width="12.14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -192,13 +204,16 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1.1</v>
@@ -209,16 +224,19 @@
       <c r="F2" s="0" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="2" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>2.2</v>
@@ -229,16 +247,19 @@
       <c r="F3" s="0" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="2" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>3.29999977111816</v>
@@ -249,16 +270,19 @@
       <c r="F4" s="0" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>4.39999771118164</v>
@@ -269,16 +293,19 @@
       <c r="F5" s="0" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="2" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>5.5</v>
@@ -289,16 +316,19 @@
       <c r="F6" s="0" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="2" t="n">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>6.6</v>
@@ -309,16 +339,16 @@
       <c r="F7" s="0" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="2" t="n">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0">
-        <v/>
-      </c>
       <c r="C8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>7.7</v>
@@ -329,16 +359,19 @@
       <c r="F8" s="0" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="2" t="n">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>8.8</v>
@@ -349,16 +382,19 @@
       <c r="F9" s="0" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="2" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>9.9</v>
@@ -369,8 +405,11 @@
       <c r="F10" s="0" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="2" t="n">
+        <v>2.45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
@@ -378,7 +417,7 @@
         <v>433</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>10.1</v>
@@ -389,16 +428,19 @@
       <c r="F11" s="0" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="2" t="n">
+        <v>1021.56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>11.11</v>
@@ -409,15 +451,18 @@
       <c r="F12" s="0" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="2" t="n">
+        <v>202.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="D13" s="3" t="n">
         <v>12.22</v>
       </c>
       <c r="E13" s="1" t="n">
@@ -425,6 +470,17 @@
       </c>
       <c r="F13" s="0" t="b">
         <v>0</v>
+      </c>
+      <c r="G13" s="4" t="n">
+        <v>33.223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="F14" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Support field data type ftLargeInt
</commit_message>
<xml_diff>
--- a/demos/TestData.xlsx
+++ b/demos/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve">AutoIncCol</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">StringCol5</t>
   </si>
   <si>
+    <t xml:space="preserve">MemoCol</t>
+  </si>
+  <si>
     <t xml:space="preserve">FloatCol</t>
   </si>
   <si>
@@ -44,6 +47,12 @@
   </si>
   <si>
     <t xml:space="preserve">CurrencyCol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text 1</t>
   </si>
   <si>
     <t xml:space="preserve">abc</t>
@@ -114,8 +123,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00&quot; &quot;[$€];&quot;-&quot;#,##0.00&quot; &quot;[$€]"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;[$€];&quot;-&quot;#,##0.00&quot; &quot;[$€]"/>
+    <numFmt numFmtId="165" formatCode="0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -159,11 +168,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" xfId="0"/>
+    <xf numFmtId="14" applyNumberFormat="1" fontId="0" xfId="0"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="0" xfId="0"/>
-    <xf numFmtId="14" applyNumberFormat="1" fontId="0" xfId="0"/>
-    <xf numFmtId="7" applyNumberFormat="1" fontId="0" xfId="0"/>
     <xf numFmtId="165" applyNumberFormat="1" fontId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -176,10 +184,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1" rightToLeft="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.14" defaultRowHeight="15.00" customHeight="true"/>
@@ -191,12 +199,13 @@
     <col min="5" max="5" width="9.14"/>
     <col min="6" max="6" width="9.14"/>
     <col min="7" max="7" width="9.14"/>
-    <col min="8" max="8" width="20.14" customWidth="1"/>
-    <col min="9" max="9" width="9.14"/>
-    <col min="10" max="10" width="12.14" customWidth="1"/>
+    <col min="8" max="8" width="9.14"/>
+    <col min="9" max="9" width="20.14" customWidth="1"/>
+    <col min="10" max="10" width="9.14"/>
+    <col min="11" max="11" width="12.14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -227,28 +236,40 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="0" t="n">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="G2" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="0" t="n">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="G3" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="G4" s="3" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="0" t="n">
         <v>1</v>
       </c>
@@ -259,25 +280,25 @@
         <v>65535</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="H6" s="0" t="n">
         <v>1.1</v>
       </c>
-      <c r="H6" s="2" t="n">
+      <c r="I6" s="1" t="n">
         <v>44228</v>
       </c>
-      <c r="I6" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="4" t="n">
+      <c r="J6" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="n">
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="0" t="n">
         <v>2</v>
       </c>
@@ -291,25 +312,25 @@
         <v>9</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="H7" s="0" t="n">
         <v>2.2</v>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="I7" s="1" t="n">
         <v>44229</v>
       </c>
-      <c r="I7" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="J7" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="0" t="n">
         <v>3</v>
       </c>
@@ -323,25 +344,25 @@
         <v>0</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="H8" s="0" t="n">
         <v>3.29999977111816</v>
       </c>
-      <c r="H8" s="2" t="n">
+      <c r="I8" s="1" t="n">
         <v>44230</v>
       </c>
-      <c r="I8" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" s="4" t="n">
+      <c r="J8" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2" t="n">
         <v>-1000</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="0" t="n">
         <v>4</v>
       </c>
@@ -355,25 +376,25 @@
         <v>567</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H9" s="0" t="n">
         <v>4.39999771118164</v>
       </c>
-      <c r="H9" s="2" t="n">
+      <c r="I9" s="1" t="n">
         <v>44231</v>
       </c>
-      <c r="I9" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="4" t="n">
+      <c r="J9" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2" t="n">
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" s="0" t="n">
         <v>5</v>
       </c>
@@ -387,25 +408,25 @@
         <v>56757</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="H10" s="0" t="n">
         <v>5.5</v>
       </c>
-      <c r="H10" s="2" t="n">
+      <c r="I10" s="1" t="n">
         <v>44597</v>
       </c>
-      <c r="I10" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" s="4" t="n">
+      <c r="J10" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="n">
         <v>33.223</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="0" t="n">
         <v>6</v>
       </c>
@@ -419,25 +440,25 @@
         <v>4564</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="H11" s="0" t="n">
         <v>6.6</v>
       </c>
-      <c r="H11" s="2" t="n">
+      <c r="I11" s="1" t="n">
         <v>44233</v>
       </c>
-      <c r="I11" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" s="4" t="n">
+      <c r="J11" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2" t="n">
         <v>452.5</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" s="0" t="n">
         <v>7</v>
       </c>
@@ -451,22 +472,22 @@
         <v>345</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="H12" s="0" t="n">
         <v>7.7</v>
       </c>
-      <c r="H12" s="2" t="n">
+      <c r="I12" s="1" t="n">
         <v>44234</v>
       </c>
-      <c r="I12" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" s="4" t="n">
+      <c r="J12" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2" t="n">
         <v>999.99</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" s="0" t="n">
         <v>8</v>
       </c>
@@ -480,25 +501,25 @@
         <v>23</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="H13" s="0" t="n">
         <v>8.8</v>
       </c>
-      <c r="H13" s="2" t="n">
+      <c r="I13" s="1" t="n">
         <v>44235</v>
       </c>
-      <c r="I13" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" s="4" t="n">
+      <c r="J13" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2" t="n">
         <v>84563.21</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" s="0" t="n">
         <v>9</v>
       </c>
@@ -509,25 +530,25 @@
         <v>12</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="H14" s="0" t="n">
         <v>9.9</v>
       </c>
-      <c r="H14" s="2" t="n">
+      <c r="I14" s="1" t="n">
         <v>44236</v>
       </c>
-      <c r="I14" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" s="4" t="n">
+      <c r="J14" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2" t="n">
         <v>33.223</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" s="0" t="n">
         <v>10</v>
       </c>
@@ -544,22 +565,22 @@
         <v>433</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="H15" s="0" t="n">
         <v>10.1</v>
       </c>
-      <c r="H15" s="2" t="n">
+      <c r="I15" s="1" t="n">
         <v>44237</v>
       </c>
-      <c r="I15" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="4" t="n">
+      <c r="J15" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2" t="n">
         <v>443.98</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" s="0" t="n">
         <v>11</v>
       </c>
@@ -570,25 +591,25 @@
         <v>-23</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="H16" s="0" t="n">
         <v>11.11</v>
       </c>
-      <c r="H16" s="2" t="n">
+      <c r="I16" s="1" t="n">
         <v>44238</v>
       </c>
-      <c r="I16" s="0" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" s="4" t="n">
+      <c r="J16" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2" t="n">
         <v>12.98</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:11">
       <c r="A17" s="0" t="n">
         <v>12</v>
       </c>
@@ -602,18 +623,18 @@
         <v>23</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="H17" s="0" t="n">
         <v>12.22</v>
       </c>
-      <c r="H17" s="2" t="n">
+      <c r="I17" s="1" t="n">
         <v>44239</v>
       </c>
-      <c r="I17" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" s="4" t="n">
+      <c r="J17" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2" t="n">
         <v>21.99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update sample data file to new field types.
</commit_message>
<xml_diff>
--- a/demos/TestData.xlsx
+++ b/demos/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prog_Lazarus\wp-git\FPSpreadsheetDataset\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5ED21274-B0AB-4ED8-AA70-92DFB63FE1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79BEFCC-1A92-4E38-94C4-B6EC68A9DFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10620" yWindow="510" windowWidth="24930" windowHeight="13545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,11 @@
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>AutoIncCol</t>
   </si>
@@ -114,6 +113,24 @@
   </si>
   <si>
     <t>tzuio</t>
+  </si>
+  <si>
+    <t>WideStringCol</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>123adf</t>
+  </si>
+  <si>
+    <t>dfsf</t>
+  </si>
+  <si>
+    <t>äöü</t>
+  </si>
+  <si>
+    <t>äöüß</t>
   </si>
 </sst>
 </file>
@@ -491,20 +508,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="3" max="4" width="11" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -524,39 +542,51 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>1</v>
       </c>
@@ -572,20 +602,23 @@
       <c r="F6" t="s">
         <v>11</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>44228</v>
       </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>2</v>
       </c>
@@ -604,20 +637,23 @@
       <c r="F7" t="s">
         <v>13</v>
       </c>
-      <c r="G7">
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>44229</v>
       </c>
-      <c r="I7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" s="2">
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>3</v>
       </c>
@@ -636,20 +672,23 @@
       <c r="F8" t="s">
         <v>15</v>
       </c>
-      <c r="G8">
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8">
         <v>3.2999997711181601</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>44230</v>
       </c>
-      <c r="I8" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" s="2">
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2">
         <v>-1000</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>4</v>
       </c>
@@ -668,20 +707,20 @@
       <c r="F9" t="s">
         <v>17</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>4.3999977111816397</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>44231</v>
       </c>
-      <c r="I9" t="b">
+      <c r="J9" t="b">
         <v>0</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>5</v>
       </c>
@@ -700,20 +739,20 @@
       <c r="F10" t="s">
         <v>19</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>5.5</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>44597</v>
       </c>
-      <c r="I10" t="b">
+      <c r="J10" t="b">
         <v>0</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K10" s="2">
         <v>33.222999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>6</v>
       </c>
@@ -732,20 +771,20 @@
       <c r="F11" t="s">
         <v>21</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>6.6</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>44233</v>
       </c>
-      <c r="I11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" s="2">
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2">
         <v>452.5</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>7</v>
       </c>
@@ -761,20 +800,20 @@
       <c r="F12" t="s">
         <v>22</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>7.7</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>44234</v>
       </c>
-      <c r="I12" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" s="2">
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2">
         <v>999.99</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>8</v>
       </c>
@@ -793,20 +832,20 @@
       <c r="F13" t="s">
         <v>24</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>8.8000000000000007</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>44235</v>
       </c>
-      <c r="I13" t="b">
+      <c r="J13" t="b">
         <v>0</v>
       </c>
-      <c r="J13" s="2">
+      <c r="K13" s="2">
         <v>84563.21</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>9</v>
       </c>
@@ -822,20 +861,20 @@
       <c r="F14" t="s">
         <v>26</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>9.9</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>44236</v>
       </c>
-      <c r="I14" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" s="2">
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2">
         <v>33.222999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>10</v>
       </c>
@@ -854,20 +893,20 @@
       <c r="F15" t="s">
         <v>27</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>10.1</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>44237</v>
       </c>
-      <c r="I15" t="b">
+      <c r="J15" t="b">
         <v>0</v>
       </c>
-      <c r="J15" s="2">
+      <c r="K15" s="2">
         <v>443.98</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>11</v>
       </c>
@@ -883,20 +922,20 @@
       <c r="F16" t="s">
         <v>29</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>11.11</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>44238</v>
       </c>
-      <c r="I16" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" s="2">
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2">
         <v>12.98</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>12</v>
       </c>
@@ -912,16 +951,16 @@
       <c r="F17" t="s">
         <v>30</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>12.22</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>44239</v>
       </c>
-      <c r="I17" t="b">
+      <c r="J17" t="b">
         <v>0</v>
       </c>
-      <c r="J17" s="2">
+      <c r="K17" s="2">
         <v>21.99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix auto-conversion of text cells to UTF8-encoded string fields (rather than widestring fields).
</commit_message>
<xml_diff>
--- a/demos/TestData.xlsx
+++ b/demos/TestData.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">CurrencyCol</t>
   </si>
   <si>
-    <t xml:space="preserve">def</t>
+    <t xml:space="preserve">def45678</t>
   </si>
   <si>
     <t xml:space="preserve">23</t>
@@ -148,7 +148,7 @@
     <t xml:space="preserve">xvw</t>
   </si>
   <si>
-    <t xml:space="preserve">äöü</t>
+    <t xml:space="preserve">äöü45678</t>
   </si>
   <si>
     <t xml:space="preserve">tzuio</t>
@@ -161,9 +161,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="#,##0.00&quot; &quot;[$€];&quot;-&quot;#,##0.00&quot; &quot;[$€]"/>
+    <numFmt numFmtId="166" formatCode="dd.mm.yyyy hh:mm"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -207,11 +208,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" xfId="0"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="0" xfId="0"/>
     <xf numFmtId="14" applyNumberFormat="1" fontId="0" xfId="0"/>
     <xf numFmtId="165" applyNumberFormat="1" fontId="0" xfId="0"/>
+    <xf numFmtId="166" applyNumberFormat="1" fontId="0" xfId="0"/>
+    <xf numFmtId="7" applyNumberFormat="1" fontId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -308,16 +311,16 @@
       <c r="H2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="I2" s="0" t="n">
         <v>2.2</v>
       </c>
-      <c r="J2" s="2" t="n">
+      <c r="J2" s="4" t="n">
         <v>44229</v>
       </c>
       <c r="K2" s="0" t="b">
         <v>1</v>
       </c>
-      <c r="L2" s="3" t="n">
+      <c r="L2" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -688,16 +691,16 @@
       <c r="H12" s="0">
         <v/>
       </c>
-      <c r="I12" s="1" t="n">
+      <c r="I12" s="0" t="n">
         <v>12.22</v>
       </c>
-      <c r="J12" s="2" t="n">
+      <c r="J12" s="4" t="n">
         <v>44239</v>
       </c>
       <c r="K12" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="L12" s="3" t="n">
+      <c r="L12" s="5" t="n">
         <v>21.99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Support field type ftFmtBCD.
</commit_message>
<xml_diff>
--- a/demos/TestData.xlsx
+++ b/demos/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prog_Lazarus\wp-git\FPSpreadsheetDataset\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48073C12-4D6D-4B81-891A-40271EE8F8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA77704-C5B9-461B-A09A-0B34BE89390B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12720" yWindow="1230" windowWidth="24930" windowHeight="13545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>AutoIncCol</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>BCDCol</t>
+  </si>
+  <si>
+    <t>FmtBCDCol</t>
+  </si>
+  <si>
+    <t>200.24</t>
   </si>
 </sst>
 </file>
@@ -547,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
@@ -569,7 +575,7 @@
     <col min="13" max="13" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -609,8 +615,11 @@
       <c r="M1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>2</v>
       </c>
@@ -650,8 +659,11 @@
       <c r="M2">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3">
         <v>3</v>
       </c>
@@ -691,8 +703,11 @@
       <c r="M3">
         <v>1000.12</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4">
         <v>4</v>
       </c>
@@ -732,8 +747,11 @@
       <c r="M4">
         <v>-2002.3434999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4">
+        <v>-4000.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5">
         <v>5</v>
       </c>
@@ -770,8 +788,11 @@
       <c r="M5">
         <v>100.95</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5">
+        <v>200.91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6">
         <v>6</v>
       </c>
@@ -808,8 +829,11 @@
       <c r="M6">
         <v>1000</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7">
         <v>7</v>
       </c>
@@ -846,8 +870,11 @@
       <c r="M7">
         <v>2000</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8">
         <v>8</v>
       </c>
@@ -885,8 +912,11 @@
       <c r="M8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9">
         <v>9</v>
       </c>
@@ -923,8 +953,11 @@
       <c r="M9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10">
         <v>10</v>
       </c>
@@ -958,8 +991,11 @@
       <c r="M10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11">
         <v>11</v>
       </c>
@@ -993,8 +1029,11 @@
       <c r="M11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1030,6 +1069,9 @@
       </c>
       <c r="M12">
         <v>5</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>